<commit_message>
Working through the institutes
</commit_message>
<xml_diff>
--- a/11-CollaborationList/2024-10-08-LhARA-list.xlsx
+++ b/11-CollaborationList/2024-10-08-LhARA-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A011A-C826-7C40-AB61-1D82C94058E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CB019F-8AC7-CE47-9A35-54508AD3D825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="546">
   <si>
     <t>Title</t>
   </si>
@@ -755,9 +755,6 @@
   </si>
   <si>
     <t>Imperial College London, CRUK PPI group, Charing Cross Hospital, London W6 8RF</t>
-  </si>
-  <si>
-    <t>Public Involvement Advisor or just plain Member of the Public</t>
   </si>
   <si>
     <t>Emma</t>
@@ -1720,6 +1717,28 @@
   </si>
   <si>
     <t>08Oct24: need to add.</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Amos</t>
+  </si>
+  <si>
+    <t>r.amos@ucl.ac.uk</t>
+  </si>
+  <si>
+    <t>R.Amos</t>
+  </si>
+  <si>
+    <t>??-USA</t>
+  </si>
+  <si>
+    <t>WPM WPA</t>
+  </si>
+  <si>
+    <t>08Oct24: refresh email sent.
+Public Involvement Advisor or just plain Member of the Public</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2257,6 +2276,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2303,7 +2335,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2327,9 +2359,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2363,6 +2392,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2480,28 +2515,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69C39425-8FEC-5B4B-8EC1-E12B4427444B}" name="Table1" displayName="Table1" ref="A1:P85" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P85" xr:uid="{69C39425-8FEC-5B4B-8EC1-E12B4427444B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P85">
-    <sortCondition ref="G1:G85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69C39425-8FEC-5B4B-8EC1-E12B4427444B}" name="Table1" displayName="Table1" ref="A1:P86" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:P86" xr:uid="{69C39425-8FEC-5B4B-8EC1-E12B4427444B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P86">
+    <sortCondition ref="G1:G86"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{737B9793-3401-7C4D-87AE-EEAD7B57BCC7}" name="Title" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{03137E78-45FB-B44B-8482-0B8AA1F52C44}" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A5F12378-6670-C347-8013-0F2F41650159}" name="Surname" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{0A4865E7-FFCA-AF48-96A1-E1298D8A03E3}" name="Initials" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{6AA70C83-D916-284F-B016-0812EFF2600C}" name="email address" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{F92E9356-55F5-0F46-A0E8-7684FDD3D01B}" name="Name on Publications " dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{07A68EBE-898B-3540-8045-C94746C529DF}" name="Organisation" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{6EFF6114-BC0E-B849-8E1E-C9359C4226E5}" name="Address" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{78903F40-B886-9249-9C0E-FFE879A550EB}" name="Number of affiliations" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{8B1BF563-D956-C34F-B2BB-B18EBB859545}" name="Affiliation code" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{86A6AEA8-2AF7-6242-A045-EE44C352E738}" name="Affiliation address" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{E28A650D-5C68-7347-9908-6F2FFED91AAE}" name="Affiliation code2" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{97CD75B8-1381-5347-8E1F-7AED39B3C00D}" name="Affiliation address3" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{6EACD8A1-1336-FD4E-A400-3098BD1784DE}" name="ORCID " dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{2E69CF99-4872-2247-9B0B-ABE8233C4E4C}" name="Role" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{61605461-4984-5E42-94D2-819418ED61AF}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{737B9793-3401-7C4D-87AE-EEAD7B57BCC7}" name="Title" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{03137E78-45FB-B44B-8482-0B8AA1F52C44}" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{A5F12378-6670-C347-8013-0F2F41650159}" name="Surname" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{0A4865E7-FFCA-AF48-96A1-E1298D8A03E3}" name="Initials" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{6AA70C83-D916-284F-B016-0812EFF2600C}" name="email address" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F92E9356-55F5-0F46-A0E8-7684FDD3D01B}" name="Name on Publications " dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{07A68EBE-898B-3540-8045-C94746C529DF}" name="Organisation" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{6EFF6114-BC0E-B849-8E1E-C9359C4226E5}" name="Address" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{78903F40-B886-9249-9C0E-FFE879A550EB}" name="Number of affiliations" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{8B1BF563-D956-C34F-B2BB-B18EBB859545}" name="Affiliation code" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{86A6AEA8-2AF7-6242-A045-EE44C352E738}" name="Affiliation address" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{E28A650D-5C68-7347-9908-6F2FFED91AAE}" name="Affiliation code2" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{97CD75B8-1381-5347-8E1F-7AED39B3C00D}" name="Affiliation address3" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{6EACD8A1-1336-FD4E-A400-3098BD1784DE}" name="ORCID " dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{2E69CF99-4872-2247-9B0B-ABE8233C4E4C}" name="Role" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{61605461-4984-5E42-94D2-819418ED61AF}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2804,13 +2839,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2878,7 +2913,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>14</v>
@@ -2889,75 +2924,75 @@
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="R2" s="19"/>
+        <v>536</v>
+      </c>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="R3" s="19"/>
+        <v>537</v>
+      </c>
+      <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -2967,30 +3002,30 @@
         <v>135</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="R4" s="19"/>
+        <v>536</v>
+      </c>
+      <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -3000,9 +3035,9 @@
         <v>70</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="R5" s="20"/>
+        <v>538</v>
+      </c>
+      <c r="R5" s="19"/>
     </row>
     <row r="6" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -3033,539 +3068,585 @@
         <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="R6" s="18"/>
     </row>
     <row r="7" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>157</v>
+        <v>539</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>158</v>
+        <v>540</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>159</v>
+        <v>541</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>160</v>
+        <v>542</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>161</v>
+        <v>51</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="J7" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="R7" s="19"/>
     </row>
     <row r="8" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>447</v>
+        <v>157</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>448</v>
+        <v>158</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>449</v>
+        <v>113</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>450</v>
+        <v>159</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>451</v>
+        <v>160</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="R8" s="18"/>
     </row>
     <row r="9" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>320</v>
+        <v>446</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>321</v>
+        <v>447</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>261</v>
+        <v>448</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>322</v>
+        <v>449</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>323</v>
+        <v>450</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>324</v>
+        <v>85</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>325</v>
+        <v>86</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
       </c>
+      <c r="N9" s="20"/>
       <c r="O9" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="R9" s="18"/>
     </row>
     <row r="10" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>517</v>
+        <v>319</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>518</v>
+        <v>320</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>260</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>519</v>
+        <v>321</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>520</v>
+        <v>322</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>522</v>
+        <v>324</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="R10" s="18"/>
     </row>
     <row r="11" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>234</v>
+        <v>516</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>235</v>
+        <v>517</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>529</v>
+        <v>81</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>518</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>237</v>
+        <v>519</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>238</v>
+        <v>520</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>239</v>
+        <v>521</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>240</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="R11" s="18"/>
     </row>
     <row r="12" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>216</v>
+        <v>236</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>528</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="R12" s="18"/>
     </row>
     <row r="13" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>362</v>
+        <v>213</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>363</v>
+        <v>214</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>364</v>
+        <v>215</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>365</v>
+        <v>216</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>366</v>
+        <v>217</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>367</v>
+        <v>218</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>368</v>
+        <v>219</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
+      <c r="O13" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="R13" s="18"/>
     </row>
     <row r="14" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>432</v>
+        <v>361</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>433</v>
+        <v>362</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>363</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>434</v>
+        <v>364</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>435</v>
+        <v>365</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="P14" s="21" t="s">
         <v>536</v>
       </c>
+      <c r="R14" s="18"/>
     </row>
     <row r="15" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>431</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>432</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>433</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>46</v>
+        <v>434</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>47</v>
+        <v>366</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>48</v>
+        <v>367</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="O15" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="31" x14ac:dyDescent="0.2">
+        <v>535</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>241</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>242</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>530</v>
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>244</v>
+        <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>245</v>
+        <v>48</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
       </c>
-      <c r="N16" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>534</v>
-      </c>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="N16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="31" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>379</v>
+        <v>240</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>380</v>
+        <v>241</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>382</v>
+        <v>242</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>529</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>383</v>
+        <v>243</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>48</v>
+        <v>244</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="N17" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>459</v>
+        <v>378</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>460</v>
+        <v>379</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>461</v>
+        <v>380</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>462</v>
+        <v>381</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>463</v>
+        <v>382</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>464</v>
+        <v>47</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>465</v>
+        <v>48</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="P18" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>337</v>
+        <v>458</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>338</v>
+        <v>459</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>54</v>
+        <v>460</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>339</v>
+        <v>461</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>340</v>
+        <v>462</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>341</v>
+        <v>463</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>342</v>
+        <v>464</v>
       </c>
       <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>430</v>
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>424</v>
+        <v>336</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>425</v>
+        <v>337</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>426</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>427</v>
+        <v>338</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>428</v>
+        <v>339</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>423</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>424</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>425</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>426</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>29</v>
+        <v>427</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>30</v>
+        <v>340</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>31</v>
+        <v>341</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>301</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>302</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>303</v>
+        <v>27</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>304</v>
+        <v>28</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>305</v>
+        <v>29</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>306</v>
+        <v>31</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -3573,25 +3654,25 @@
         <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>300</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>456</v>
+        <v>301</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>229</v>
+        <v>302</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>457</v>
+        <v>303</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>458</v>
+        <v>304</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -3602,87 +3683,87 @@
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>343</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>492</v>
+        <v>455</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>493</v>
+        <v>456</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>494</v>
+        <v>457</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>31</v>
+        <v>305</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
       </c>
-      <c r="N24" s="17"/>
-      <c r="O24" s="1" t="s">
-        <v>534</v>
-      </c>
     </row>
     <row r="25" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>342</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>491</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>152</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>153</v>
+        <v>492</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>154</v>
+        <v>493</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>155</v>
+        <v>30</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>156</v>
+        <v>31</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="N25" s="16"/>
+      <c r="O25" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>290</v>
+        <v>150</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>291</v>
+        <v>151</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>292</v>
+        <v>152</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>293</v>
+        <v>153</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>294</v>
+        <v>154</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>155</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>295</v>
+        <v>156</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -3690,540 +3771,534 @@
     </row>
     <row r="27" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
+        <v>291</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>155</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>344</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>346</v>
+        <v>297</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>155</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>169</v>
+        <v>294</v>
       </c>
       <c r="I28" s="1">
         <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>317</v>
+        <v>30</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>410</v>
+        <v>343</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>411</v>
+        <v>344</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>413</v>
+        <v>345</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>155</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>295</v>
+        <v>169</v>
       </c>
       <c r="I29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>155</v>
+        <v>316</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>31</v>
+        <v>317</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>487</v>
+        <v>409</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>488</v>
+        <v>410</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>489</v>
+        <v>411</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>490</v>
+        <v>412</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>155</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I31" s="1">
         <v>0</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="K31" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>534</v>
+        <v>490</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>495</v>
+        <v>120</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>496</v>
+        <v>122</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>497</v>
+        <v>123</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>498</v>
+        <v>124</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>499</v>
+        <v>125</v>
       </c>
       <c r="I32" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>401</v>
+        <v>190</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>402</v>
+        <v>494</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>403</v>
+        <v>62</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>404</v>
+        <v>495</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>405</v>
+        <v>496</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>406</v>
+        <v>497</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>407</v>
+        <v>498</v>
       </c>
       <c r="I33" s="1">
-        <v>1</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>534</v>
-      </c>
     </row>
     <row r="36" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>201</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>202</v>
+        <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>203</v>
+        <v>55</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>204</v>
+        <v>56</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>205</v>
+        <v>57</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>201</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>130</v>
+        <v>62</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="I37" s="1">
         <v>0</v>
       </c>
-      <c r="K37" s="6"/>
-      <c r="N37" s="1" t="s">
-        <v>134</v>
+      <c r="O37" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>183</v>
+        <v>128</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>184</v>
+        <v>129</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="13" t="s">
-        <v>185</v>
+      <c r="E38" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>524</v>
+        <v>131</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>187</v>
+        <v>133</v>
       </c>
       <c r="I38" s="1">
-        <v>1</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="6"/>
+      <c r="N38" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>223</v>
+        <v>27</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>224</v>
+        <v>523</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>186</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="I39" s="1">
-        <v>0</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="O39" s="8"/>
-    </row>
-    <row r="40" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>439</v>
+        <v>220</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>440</v>
+        <v>221</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>442</v>
+        <v>222</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>443</v>
+        <v>224</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>444</v>
+        <v>186</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>445</v>
+        <v>225</v>
       </c>
       <c r="I40" s="1">
         <v>0</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>534</v>
-      </c>
+      <c r="N40" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="O40" s="8"/>
     </row>
     <row r="41" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>111</v>
+        <v>438</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>112</v>
+        <v>439</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>113</v>
+        <v>440</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>114</v>
+        <v>441</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>115</v>
+        <v>442</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>116</v>
+        <v>443</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>117</v>
+        <v>444</v>
       </c>
       <c r="I41" s="1">
         <v>0</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>118</v>
+        <v>445</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>396</v>
+        <v>111</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>397</v>
+        <v>112</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>229</v>
+        <v>113</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>398</v>
+        <v>114</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>399</v>
+        <v>115</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>116</v>
@@ -4235,42 +4310,42 @@
         <v>0</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>400</v>
+        <v>118</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>395</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>17</v>
+        <v>396</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>18</v>
+        <v>229</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>19</v>
+        <v>397</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>20</v>
+        <v>398</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>534</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -4278,19 +4353,19 @@
         <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>286</v>
+        <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>287</v>
+        <v>17</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>288</v>
+        <v>19</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>289</v>
+        <v>20</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>21</v>
@@ -4301,28 +4376,31 @@
       <c r="I44" s="1">
         <v>0</v>
       </c>
+      <c r="N44" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="O44" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>436</v>
+        <v>285</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>433</v>
+        <v>286</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>437</v>
+        <v>287</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>438</v>
+        <v>288</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>21</v>
@@ -4334,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -4342,19 +4420,19 @@
         <v>33</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>509</v>
+        <v>435</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>510</v>
+        <v>432</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>229</v>
+        <v>54</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>511</v>
+        <v>436</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>512</v>
+        <v>437</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>21</v>
@@ -4364,6 +4442,9 @@
       </c>
       <c r="I46" s="1">
         <v>0</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -4371,60 +4452,54 @@
         <v>33</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>508</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>164</v>
+        <v>509</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>166</v>
+        <v>510</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>167</v>
+        <v>511</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>168</v>
+        <v>21</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I48" s="1">
         <v>1</v>
@@ -4433,63 +4508,62 @@
         <v>155</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>254</v>
+        <v>170</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>255</v>
+        <v>171</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>256</v>
+        <v>173</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="I49" s="1">
-        <v>0</v>
-      </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-    </row>
-    <row r="50" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>258</v>
+        <v>33</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>261</v>
+        <v>27</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>168</v>
@@ -4498,39 +4572,34 @@
         <v>169</v>
       </c>
       <c r="I50" s="1">
-        <v>1</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
     </row>
     <row r="51" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>257</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>307</v>
+        <v>258</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>308</v>
+        <v>259</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>309</v>
+        <v>260</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>310</v>
+        <v>261</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>311</v>
+        <v>262</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>168</v>
@@ -4539,86 +4608,95 @@
         <v>169</v>
       </c>
       <c r="I51" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I52" s="1">
-        <v>2</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>523</v>
+        <v>312</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>531</v>
+        <v>313</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="I53" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>329</v>
+        <v>318</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -4626,54 +4704,51 @@
         <v>68</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>348</v>
+        <v>522</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>532</v>
+        <v>326</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>530</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I54" s="1">
-        <v>1</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>376</v>
+        <v>531</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>168</v>
@@ -4685,36 +4760,30 @@
         <v>1</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>155</v>
+        <v>340</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>534</v>
+        <v>350</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>420</v>
+        <v>372</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>421</v>
+        <v>373</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>44</v>
+        <v>374</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>422</v>
+        <v>375</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>423</v>
+        <v>376</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>168</v>
@@ -4723,39 +4792,39 @@
         <v>175</v>
       </c>
       <c r="I56" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>155</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>478</v>
+        <v>419</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>479</v>
+        <v>420</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>480</v>
+        <v>44</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>481</v>
+        <v>421</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>482</v>
+        <v>422</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>168</v>
@@ -4763,146 +4832,155 @@
       <c r="H57" s="1" t="s">
         <v>175</v>
       </c>
+      <c r="I57" s="1">
+        <v>2</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="58" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>477</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
+        <v>478</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>97</v>
+        <v>479</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>98</v>
+        <v>481</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I58" s="1">
-        <v>1</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>102</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>201</v>
+        <v>94</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>385</v>
+        <v>95</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>387</v>
+        <v>96</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>388</v>
+        <v>98</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>389</v>
+        <v>100</v>
       </c>
       <c r="I59" s="1">
-        <v>0</v>
-      </c>
-      <c r="N59" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="O59" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="60" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>452</v>
+        <v>201</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>453</v>
+        <v>384</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>454</v>
+        <v>385</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>386</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>455</v>
+        <v>387</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>100</v>
+        <v>388</v>
       </c>
       <c r="I60" s="1">
-        <v>1</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>534</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N60" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="O60" s="10"/>
     </row>
     <row r="61" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>207</v>
+        <v>451</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>208</v>
+        <v>452</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>209</v>
+        <v>453</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>210</v>
+        <v>454</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>211</v>
+        <v>99</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>212</v>
+        <v>100</v>
       </c>
       <c r="I61" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -4910,19 +4988,19 @@
         <v>15</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>452</v>
+        <v>207</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>500</v>
+        <v>208</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>501</v>
+        <v>209</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>502</v>
+        <v>210</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>211</v>
@@ -4932,6 +5010,9 @@
       </c>
       <c r="I62" s="1">
         <v>0</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -4939,19 +5020,19 @@
         <v>15</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>503</v>
+        <v>451</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>505</v>
+        <v>18</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>211</v>
@@ -4960,42 +5041,33 @@
         <v>212</v>
       </c>
       <c r="I63" s="1">
-        <v>1</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N63" s="1" t="s">
-        <v>508</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>69</v>
+        <v>502</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>70</v>
+        <v>503</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>71</v>
+        <v>504</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>72</v>
+        <v>505</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>73</v>
+        <v>506</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>75</v>
+        <v>212</v>
       </c>
       <c r="I64" s="1">
         <v>1</v>
@@ -5007,107 +5079,107 @@
         <v>77</v>
       </c>
       <c r="N64" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N65" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
+    <row r="66" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B66" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="C66" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="D66" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E65" s="15" t="s">
+      <c r="F66" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="G66" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="H66" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="G65" s="14" t="s">
+      <c r="I66" s="13">
+        <v>1</v>
+      </c>
+      <c r="J66" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="H65" s="14" t="s">
+      <c r="K66" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="I65" s="14">
-        <v>1</v>
-      </c>
-      <c r="J65" s="14" t="s">
-        <v>526</v>
-      </c>
-      <c r="K65" s="14" t="s">
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="O65" s="16"/>
-      <c r="P65" s="14"/>
-    </row>
-    <row r="66" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I66" s="1">
-        <v>1</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O66" s="1" t="s">
-        <v>534</v>
-      </c>
+      <c r="O66" s="15"/>
+      <c r="P66" s="13"/>
     </row>
     <row r="67" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>190</v>
+        <v>103</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>191</v>
+        <v>104</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>528</v>
+      <c r="E67" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>107</v>
@@ -5122,229 +5194,235 @@
         <v>109</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="N67" s="1" t="s">
-        <v>194</v>
+        <v>110</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>69</v>
+        <v>190</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>475</v>
+        <v>191</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>476</v>
+        <v>62</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>527</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>477</v>
+        <v>192</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>107</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I68" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>466</v>
+        <v>69</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>468</v>
+        <v>71</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>471</v>
+        <v>107</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>472</v>
+        <v>110</v>
       </c>
       <c r="I69" s="1">
-        <v>1</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="K69" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="O69" s="1" t="s">
-        <v>534</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>34</v>
+        <v>465</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>35</v>
+        <v>466</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>36</v>
+        <v>467</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>37</v>
+        <v>468</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>38</v>
+        <v>469</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>39</v>
+        <v>470</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>40</v>
+        <v>471</v>
       </c>
       <c r="I70" s="1">
-        <v>0</v>
-      </c>
-      <c r="N70" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
       </c>
-      <c r="O71" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="N71" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>179</v>
+        <v>113</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="7" t="s">
-        <v>181</v>
+      <c r="H72" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="I72" s="1">
         <v>0</v>
       </c>
-      <c r="N72" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="O72" s="7"/>
-    </row>
-    <row r="73" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="O72" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>228</v>
+        <v>178</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>230</v>
+        <v>62</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>179</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>233</v>
+        <v>39</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="I73" s="1">
         <v>0</v>
       </c>
-      <c r="O73" s="1" t="s">
-        <v>534</v>
-      </c>
+      <c r="N73" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="O73" s="7"/>
     </row>
     <row r="74" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>358</v>
+        <v>227</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>359</v>
+        <v>228</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>81</v>
+        <v>229</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>360</v>
+        <v>230</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>361</v>
+        <v>231</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>232</v>
@@ -5353,165 +5431,168 @@
         <v>233</v>
       </c>
       <c r="I74" s="1">
-        <v>1</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>60</v>
+        <v>357</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>61</v>
+        <v>358</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>64</v>
+        <v>360</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>66</v>
+        <v>233</v>
       </c>
       <c r="I75" s="1">
-        <v>0</v>
-      </c>
-      <c r="N75" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O75" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="76" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>247</v>
+        <v>60</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>248</v>
+        <v>61</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>250</v>
+        <v>62</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>251</v>
+        <v>64</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>252</v>
+        <v>65</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="I76" s="1">
         <v>0</v>
       </c>
+      <c r="N76" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O76" s="7"/>
     </row>
     <row r="77" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D78" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="G78" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I78" s="1">
+        <v>1</v>
+      </c>
+      <c r="J78" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G77" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="I77" s="1">
-        <v>1</v>
-      </c>
-      <c r="J77" s="1" t="s">
+      <c r="K78" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="K77" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O77" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I78" s="1">
-        <v>0</v>
+      <c r="O78" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="79" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>92</v>
@@ -5522,28 +5603,25 @@
       <c r="I79" s="1">
         <v>0</v>
       </c>
-      <c r="O79" s="1" t="s">
-        <v>534</v>
-      </c>
     </row>
     <row r="80" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>391</v>
+        <v>140</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>392</v>
+        <v>141</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>393</v>
+        <v>44</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>394</v>
+        <v>142</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>395</v>
+        <v>143</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>92</v>
@@ -5554,145 +5632,142 @@
       <c r="I80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="O80" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>79</v>
+        <v>390</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>80</v>
+        <v>391</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>527</v>
+        <v>392</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>82</v>
+        <v>394</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="I81" s="1">
-        <v>1</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>197</v>
+      <c r="E82" s="4" t="s">
+        <v>526</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>199</v>
+        <v>84</v>
       </c>
       <c r="I82" s="1">
-        <v>0</v>
-      </c>
-      <c r="N82" s="1" t="s">
-        <v>200</v>
+        <v>1</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>352</v>
+        <v>196</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>353</v>
+        <v>81</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>354</v>
+        <v>198</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>355</v>
+        <v>199</v>
       </c>
       <c r="I83" s="1">
-        <v>1</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="O83" s="1" t="s">
-        <v>534</v>
+        <v>0</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>483</v>
+        <v>50</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>484</v>
+        <v>351</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>485</v>
+        <v>18</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>352</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>486</v>
+        <v>353</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I84" s="1">
         <v>1</v>
       </c>
       <c r="J84" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K84" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K84" s="1" t="s">
-        <v>357</v>
+      <c r="O84" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -5700,54 +5775,89 @@
         <v>33</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>513</v>
+        <v>482</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>514</v>
+        <v>483</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>515</v>
+        <v>484</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>516</v>
+        <v>485</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I85" s="1">
         <v>1</v>
       </c>
       <c r="J85" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K85" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K85" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="O85" s="1" t="s">
-        <v>536</v>
+    </row>
+    <row r="86" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="I86" s="1">
+        <v>1</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E72" r:id="rId1" xr:uid="{249EAE20-EF4B-4353-9BDD-701C738070A1}"/>
-    <hyperlink ref="E39" r:id="rId2" xr:uid="{C5A0A689-7908-4EFA-AFBA-CA0689730743}"/>
-    <hyperlink ref="E75" r:id="rId3" xr:uid="{D1CDFB7A-6BEC-48FB-834C-8CB88E5F4016}"/>
-    <hyperlink ref="E59" r:id="rId4" xr:uid="{DF5D1539-1A7C-4613-9FF0-2DA1AF9DEF8A}"/>
-    <hyperlink ref="E37" r:id="rId5" xr:uid="{0FB9BB4C-CA10-4CCE-A735-F27061753B59}"/>
-    <hyperlink ref="E38" r:id="rId6" xr:uid="{83EB2AB8-A28E-3345-84F9-2F81AE882DEE}"/>
-    <hyperlink ref="E65" r:id="rId7" xr:uid="{32EBF51D-E743-46D4-8A67-637908371B66}"/>
-    <hyperlink ref="E81" r:id="rId8" xr:uid="{D5417B78-6A2B-2549-9C05-111AB744469E}"/>
-    <hyperlink ref="E67" r:id="rId9" xr:uid="{446814EC-9402-CA42-9669-6F09EE6F1BF6}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{86E75FC4-AC95-9549-81C2-3409075C9B4D}"/>
-    <hyperlink ref="E53" r:id="rId11" xr:uid="{C56B030F-609B-E841-A28A-5C4DADA2FD3C}"/>
-    <hyperlink ref="E83" r:id="rId12" xr:uid="{1D4237E7-2348-0D46-9BF3-92C9CAF89B80}"/>
-    <hyperlink ref="E58" r:id="rId13" xr:uid="{271F36D7-77A3-EA46-A99F-EF80FF74AD34}"/>
+    <hyperlink ref="E73" r:id="rId1" xr:uid="{249EAE20-EF4B-4353-9BDD-701C738070A1}"/>
+    <hyperlink ref="E40" r:id="rId2" xr:uid="{C5A0A689-7908-4EFA-AFBA-CA0689730743}"/>
+    <hyperlink ref="E76" r:id="rId3" xr:uid="{D1CDFB7A-6BEC-48FB-834C-8CB88E5F4016}"/>
+    <hyperlink ref="E60" r:id="rId4" xr:uid="{DF5D1539-1A7C-4613-9FF0-2DA1AF9DEF8A}"/>
+    <hyperlink ref="E38" r:id="rId5" xr:uid="{0FB9BB4C-CA10-4CCE-A735-F27061753B59}"/>
+    <hyperlink ref="E39" r:id="rId6" xr:uid="{83EB2AB8-A28E-3345-84F9-2F81AE882DEE}"/>
+    <hyperlink ref="E66" r:id="rId7" xr:uid="{32EBF51D-E743-46D4-8A67-637908371B66}"/>
+    <hyperlink ref="E82" r:id="rId8" xr:uid="{D5417B78-6A2B-2549-9C05-111AB744469E}"/>
+    <hyperlink ref="E68" r:id="rId9" xr:uid="{446814EC-9402-CA42-9669-6F09EE6F1BF6}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{86E75FC4-AC95-9549-81C2-3409075C9B4D}"/>
+    <hyperlink ref="E54" r:id="rId11" xr:uid="{C56B030F-609B-E841-A28A-5C4DADA2FD3C}"/>
+    <hyperlink ref="E84" r:id="rId12" xr:uid="{1D4237E7-2348-0D46-9BF3-92C9CAF89B80}"/>
+    <hyperlink ref="E59" r:id="rId13" xr:uid="{271F36D7-77A3-EA46-A99F-EF80FF74AD34}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -5757,9 +5867,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5909,26 +6022,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A185A5-328F-43C8-941B-4ACF0BBCA09C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D201AF0C-D84D-4646-898F-B45F73A20A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d2c9d8e6-4447-41a5-9589-9fed66499f9c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5952,9 +6054,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D201AF0C-D84D-4646-898F-B45F73A20A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A185A5-328F-43C8-941B-4ACF0BBCA09C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="d2c9d8e6-4447-41a5-9589-9fed66499f9c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>